<commit_message>
Update to seed data spreadsheet
</commit_message>
<xml_diff>
--- a/BDEditor/Recommended Empiric Structure Annotated.xlsx
+++ b/BDEditor/Recommended Empiric Structure Annotated.xlsx
@@ -4,25 +4,29 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="21721"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="5360" yWindow="500" windowWidth="38180" windowHeight="20320" tabRatio="472" activeTab="3"/>
+    <workbookView xWindow="1660" yWindow="20" windowWidth="36060" windowHeight="20760" tabRatio="472" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Chapter 1" sheetId="3" r:id="rId1"/>
     <sheet name="Chapter 2a" sheetId="1" r:id="rId2"/>
-    <sheet name="Chapter 2b" sheetId="7" r:id="rId3"/>
-    <sheet name="Chapter 2c" sheetId="8" r:id="rId4"/>
-    <sheet name="Chapter 3" sheetId="2" r:id="rId5"/>
-    <sheet name="Chapter 4" sheetId="4" r:id="rId6"/>
-    <sheet name="Chapter 5" sheetId="5" r:id="rId7"/>
-    <sheet name="Chapter 6" sheetId="6" r:id="rId8"/>
+    <sheet name="Chapter 2b" sheetId="11" r:id="rId3"/>
+    <sheet name="Chapter 2c" sheetId="10" r:id="rId4"/>
+    <sheet name="Chapter 2d" sheetId="7" r:id="rId5"/>
+    <sheet name="Chapter 2e" sheetId="8" r:id="rId6"/>
+    <sheet name="Chapter 3" sheetId="2" r:id="rId7"/>
+    <sheet name="Chapter 4" sheetId="4" r:id="rId8"/>
+    <sheet name="Chapter 5" sheetId="5" r:id="rId9"/>
+    <sheet name="Chapter 6" sheetId="6" r:id="rId10"/>
+    <sheet name="Samples" sheetId="9" r:id="rId11"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm.Print_Area" localSheetId="1">'Chapter 2a'!$D$1:$G$541</definedName>
-    <definedName name="_xlnm.Print_Area" localSheetId="2">'Chapter 2b'!$D$1:$E$3</definedName>
-    <definedName name="_xlnm.Print_Area" localSheetId="3">'Chapter 2c'!$D$1:$G$2</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="4">'Chapter 2d'!$D$1:$E$2</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="5">'Chapter 2e'!$D$1:$G$2</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="10">Samples!$A$1:$G$34</definedName>
     <definedName name="_xlnm.Print_Titles" localSheetId="1">'Chapter 2a'!$1:$2</definedName>
-    <definedName name="_xlnm.Print_Titles" localSheetId="2">'Chapter 2b'!$1:$2</definedName>
-    <definedName name="_xlnm.Print_Titles" localSheetId="3">'Chapter 2c'!$1:$2</definedName>
+    <definedName name="_xlnm.Print_Titles" localSheetId="4">'Chapter 2d'!$1:$2</definedName>
+    <definedName name="_xlnm.Print_Titles" localSheetId="5">'Chapter 2e'!$1:$2</definedName>
   </definedNames>
   <calcPr calcId="140000" concurrentCalc="0"/>
   <extLst>
@@ -93,7 +97,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2230" uniqueCount="1553">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2319" uniqueCount="1557">
   <si>
     <t>Category</t>
   </si>
@@ -4775,12 +4779,24 @@
   <si>
     <t>Disease (Parasite)</t>
   </si>
+  <si>
+    <t>Treatment of Culture-proven Meningitis</t>
+  </si>
+  <si>
+    <t>Treatment of Culture - proven Endocarditis</t>
+  </si>
+  <si>
+    <t>Pathogen</t>
+  </si>
+  <si>
+    <t>Pathogen Group</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="13" x14ac:knownFonts="1">
+  <fonts count="14" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -4867,8 +4883,15 @@
       <name val="Calibri"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="16">
+  <fills count="17">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -4959,8 +4982,13 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -4968,8 +4996,19 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="medium">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="519">
+  <cellStyleXfs count="532">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -5489,8 +5528,21 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="38">
+  <cellXfs count="51">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -5572,6 +5624,33 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="11" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="16" borderId="1" xfId="519" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -5588,7 +5667,8 @@
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
-  <cellStyles count="519">
+  <cellStyles count="532">
+    <cellStyle name="Bad" xfId="519" builtinId="27"/>
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -5848,6 +5928,12 @@
     <cellStyle name="Followed Hyperlink" xfId="514" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="516" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="518" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="521" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="523" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="525" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="527" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="529" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="531" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -6107,6 +6193,12 @@
     <cellStyle name="Hyperlink" xfId="513" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="515" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="517" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="520" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="522" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="524" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="526" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="528" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="530" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -6457,13 +6549,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="24" customHeight="1">
-      <c r="A1" s="33" t="s">
+      <c r="A1" s="46" t="s">
         <v>245</v>
       </c>
-      <c r="B1" s="33"/>
-      <c r="C1" s="33"/>
-      <c r="D1" s="33"/>
-      <c r="E1" s="33"/>
+      <c r="B1" s="46"/>
+      <c r="C1" s="46"/>
+      <c r="D1" s="46"/>
+      <c r="E1" s="46"/>
     </row>
     <row r="2" spans="1:6" s="24" customFormat="1">
       <c r="A2" s="25" t="s">
@@ -8080,6 +8172,703 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr enableFormatConditionsCalculation="0">
+    <tabColor theme="6" tint="0.39997558519241921"/>
+  </sheetPr>
+  <dimension ref="A1:E54"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E41" sqref="E41"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <cols>
+    <col min="2" max="2" width="50.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.1640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="24.5" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="24" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5">
+      <c r="A1" s="8" t="s">
+        <v>268</v>
+      </c>
+      <c r="B1" s="8"/>
+      <c r="C1" s="8"/>
+      <c r="D1" s="8"/>
+    </row>
+    <row r="2" spans="1:5">
+      <c r="A2" s="21" t="s">
+        <v>241</v>
+      </c>
+      <c r="B2" s="21" t="s">
+        <v>240</v>
+      </c>
+      <c r="C2" s="21" t="s">
+        <v>735</v>
+      </c>
+      <c r="D2" s="21" t="s">
+        <v>736</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" s="16" customFormat="1">
+      <c r="A3" s="16" t="s">
+        <v>276</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5">
+      <c r="B4" t="s">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5">
+      <c r="C5" s="22" t="s">
+        <v>6</v>
+      </c>
+      <c r="D5" t="s">
+        <v>737</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5">
+      <c r="C6" s="22" t="s">
+        <v>6</v>
+      </c>
+      <c r="D6" t="s">
+        <v>738</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5">
+      <c r="C7" s="22" t="s">
+        <v>6</v>
+      </c>
+      <c r="D7" t="s">
+        <v>739</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5">
+      <c r="C8" s="22" t="s">
+        <v>6</v>
+      </c>
+      <c r="D8" t="s">
+        <v>740</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5">
+      <c r="C9" s="22" t="s">
+        <v>6</v>
+      </c>
+      <c r="D9" t="s">
+        <v>741</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5">
+      <c r="C10" s="22" t="s">
+        <v>742</v>
+      </c>
+      <c r="D10" t="s">
+        <v>743</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5">
+      <c r="C11" s="22" t="s">
+        <v>742</v>
+      </c>
+      <c r="D11" t="s">
+        <v>744</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5">
+      <c r="C12" s="22" t="s">
+        <v>742</v>
+      </c>
+      <c r="D12" t="s">
+        <v>745</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5">
+      <c r="C13" s="22" t="s">
+        <v>742</v>
+      </c>
+      <c r="D13" t="s">
+        <v>746</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5">
+      <c r="C14" s="22" t="s">
+        <v>742</v>
+      </c>
+      <c r="D14" t="s">
+        <v>747</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5">
+      <c r="C15" s="22"/>
+    </row>
+    <row r="16" spans="1:5">
+      <c r="A16" s="21" t="s">
+        <v>241</v>
+      </c>
+      <c r="B16" s="21" t="s">
+        <v>240</v>
+      </c>
+      <c r="C16" s="21" t="s">
+        <v>0</v>
+      </c>
+      <c r="D16" s="21" t="s">
+        <v>570</v>
+      </c>
+      <c r="E16" s="21" t="s">
+        <v>749</v>
+      </c>
+    </row>
+    <row r="17" spans="2:4" s="16" customFormat="1">
+      <c r="B17" s="16" t="s">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="18" spans="2:4">
+      <c r="C18" t="s">
+        <v>714</v>
+      </c>
+    </row>
+    <row r="19" spans="2:4">
+      <c r="D19" t="s">
+        <v>709</v>
+      </c>
+    </row>
+    <row r="20" spans="2:4">
+      <c r="D20" t="s">
+        <v>710</v>
+      </c>
+    </row>
+    <row r="21" spans="2:4">
+      <c r="C21" t="s">
+        <v>715</v>
+      </c>
+    </row>
+    <row r="22" spans="2:4">
+      <c r="D22" t="s">
+        <v>711</v>
+      </c>
+    </row>
+    <row r="23" spans="2:4">
+      <c r="D23" t="s">
+        <v>712</v>
+      </c>
+    </row>
+    <row r="24" spans="2:4">
+      <c r="C24" t="s">
+        <v>716</v>
+      </c>
+    </row>
+    <row r="25" spans="2:4">
+      <c r="D25" t="s">
+        <v>711</v>
+      </c>
+    </row>
+    <row r="26" spans="2:4">
+      <c r="D26" t="s">
+        <v>712</v>
+      </c>
+    </row>
+    <row r="27" spans="2:4">
+      <c r="C27" t="s">
+        <v>717</v>
+      </c>
+    </row>
+    <row r="28" spans="2:4">
+      <c r="D28" t="s">
+        <v>713</v>
+      </c>
+    </row>
+    <row r="29" spans="2:4">
+      <c r="D29" t="s">
+        <v>712</v>
+      </c>
+    </row>
+    <row r="30" spans="2:4">
+      <c r="C30" t="s">
+        <v>718</v>
+      </c>
+    </row>
+    <row r="31" spans="2:4">
+      <c r="D31" t="s">
+        <v>711</v>
+      </c>
+    </row>
+    <row r="32" spans="2:4">
+      <c r="D32" t="s">
+        <v>712</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5">
+      <c r="E33" t="s">
+        <v>721</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5">
+      <c r="E34" t="s">
+        <v>712</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5">
+      <c r="E35" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5">
+      <c r="C36" t="s">
+        <v>719</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5">
+      <c r="D37" t="s">
+        <v>720</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5">
+      <c r="D38" t="s">
+        <v>712</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5">
+      <c r="E39" t="s">
+        <v>722</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5">
+      <c r="E40" t="s">
+        <v>723</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5">
+      <c r="E41" t="s">
+        <v>724</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5">
+      <c r="A42" s="21" t="s">
+        <v>241</v>
+      </c>
+      <c r="B42" s="21" t="s">
+        <v>240</v>
+      </c>
+      <c r="C42" s="21" t="s">
+        <v>0</v>
+      </c>
+      <c r="D42" s="21"/>
+    </row>
+    <row r="43" spans="1:5" s="16" customFormat="1">
+      <c r="B43" s="16" t="s">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5">
+      <c r="C44" t="s">
+        <v>725</v>
+      </c>
+    </row>
+    <row r="45" spans="1:5">
+      <c r="C45" t="s">
+        <v>726</v>
+      </c>
+    </row>
+    <row r="46" spans="1:5">
+      <c r="C46" t="s">
+        <v>727</v>
+      </c>
+    </row>
+    <row r="47" spans="1:5">
+      <c r="C47" t="s">
+        <v>728</v>
+      </c>
+    </row>
+    <row r="48" spans="1:5">
+      <c r="C48" t="s">
+        <v>729</v>
+      </c>
+    </row>
+    <row r="49" spans="2:3">
+      <c r="C49" t="s">
+        <v>730</v>
+      </c>
+    </row>
+    <row r="50" spans="2:3">
+      <c r="C50" t="s">
+        <v>731</v>
+      </c>
+    </row>
+    <row r="51" spans="2:3">
+      <c r="C51" t="s">
+        <v>732</v>
+      </c>
+    </row>
+    <row r="52" spans="2:3">
+      <c r="C52" t="s">
+        <v>733</v>
+      </c>
+    </row>
+    <row r="54" spans="2:3" s="16" customFormat="1">
+      <c r="B54" s="16" t="s">
+        <v>275</v>
+      </c>
+      <c r="C54" s="16" t="s">
+        <v>734</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr enableFormatConditionsCalculation="0">
+    <pageSetUpPr fitToPage="1"/>
+  </sheetPr>
+  <dimension ref="A1:G34"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E30" sqref="E30"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <cols>
+    <col min="1" max="1" width="30.5" style="34" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="21.6640625" style="34" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="46.83203125" style="34" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.33203125" style="34" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="27" style="34" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="18" style="34" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="17" style="34" bestFit="1" customWidth="1"/>
+    <col min="8" max="16384" width="10.83203125" style="34"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" ht="24" customHeight="1">
+      <c r="A1" s="47" t="s">
+        <v>269</v>
+      </c>
+      <c r="B1" s="47"/>
+      <c r="C1" s="47"/>
+      <c r="D1" s="47"/>
+      <c r="E1" s="47"/>
+      <c r="F1" s="47"/>
+      <c r="G1" s="47"/>
+    </row>
+    <row r="2" spans="1:7" s="45" customFormat="1" ht="28" customHeight="1" thickBot="1">
+      <c r="A2" s="45" t="s">
+        <v>912</v>
+      </c>
+      <c r="B2" s="45" t="s">
+        <v>241</v>
+      </c>
+      <c r="C2" s="45" t="s">
+        <v>240</v>
+      </c>
+      <c r="D2" s="45" t="s">
+        <v>0</v>
+      </c>
+      <c r="E2" s="45" t="s">
+        <v>9</v>
+      </c>
+      <c r="F2" s="45" t="s">
+        <v>175</v>
+      </c>
+      <c r="G2" s="45" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" s="35" customFormat="1" ht="20" customHeight="1">
+      <c r="A3" s="36" t="s">
+        <v>888</v>
+      </c>
+      <c r="B3" s="37" t="s">
+        <v>243</v>
+      </c>
+      <c r="C3" s="38"/>
+    </row>
+    <row r="4" spans="1:7" s="39" customFormat="1" ht="20" customHeight="1">
+      <c r="A4" s="39" t="s">
+        <v>889</v>
+      </c>
+      <c r="B4" s="40"/>
+      <c r="C4" s="40" t="s">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" s="33" customFormat="1" ht="14">
+      <c r="A5" s="33" t="s">
+        <v>890</v>
+      </c>
+      <c r="D5" s="33" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" s="41" customFormat="1" ht="14">
+      <c r="A6" s="41" t="s">
+        <v>891</v>
+      </c>
+      <c r="F6" s="41" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" s="41" customFormat="1" ht="14">
+      <c r="A7" s="41" t="s">
+        <v>892</v>
+      </c>
+      <c r="G7" s="42" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" s="41" customFormat="1" ht="14">
+      <c r="A8" s="41" t="s">
+        <v>893</v>
+      </c>
+      <c r="F8" s="41" t="s">
+        <v>291</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" s="41" customFormat="1" ht="14">
+      <c r="A9" s="41" t="s">
+        <v>894</v>
+      </c>
+      <c r="G9" s="41" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" s="41" customFormat="1" ht="14">
+      <c r="A10" s="41" t="s">
+        <v>895</v>
+      </c>
+      <c r="G10" s="41" t="s">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" s="43" customFormat="1" ht="25" customHeight="1" thickBot="1">
+      <c r="A12" s="43" t="s">
+        <v>912</v>
+      </c>
+      <c r="B12" s="43" t="s">
+        <v>241</v>
+      </c>
+      <c r="C12" s="43" t="s">
+        <v>240</v>
+      </c>
+      <c r="D12" s="44" t="s">
+        <v>175</v>
+      </c>
+      <c r="E12" s="43" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" s="11" customFormat="1" ht="14">
+      <c r="A13" s="11" t="s">
+        <v>1421</v>
+      </c>
+      <c r="B13" s="12"/>
+      <c r="C13" s="12" t="s">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" s="3" customFormat="1" ht="14">
+      <c r="A14" s="3" t="s">
+        <v>1422</v>
+      </c>
+      <c r="D14" s="3" t="s">
+        <v>385</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" s="3" customFormat="1" ht="14">
+      <c r="A15" s="3" t="s">
+        <v>1423</v>
+      </c>
+      <c r="E15" s="3" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" s="3" customFormat="1" ht="14">
+      <c r="A16" s="3" t="s">
+        <v>1424</v>
+      </c>
+      <c r="D16" s="3" t="s">
+        <v>386</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" s="3" customFormat="1" ht="14">
+      <c r="A17" s="3" t="s">
+        <v>1425</v>
+      </c>
+      <c r="E17" s="3" t="s">
+        <v>387</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" s="3" customFormat="1" ht="14">
+      <c r="A18" s="3" t="s">
+        <v>1426</v>
+      </c>
+      <c r="E18" s="3" t="s">
+        <v>388</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" s="3" customFormat="1" ht="14">
+      <c r="A19" s="3" t="s">
+        <v>1427</v>
+      </c>
+      <c r="E19" s="3" t="s">
+        <v>389</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" s="43" customFormat="1" ht="28" customHeight="1" thickBot="1">
+      <c r="A21" s="43" t="s">
+        <v>912</v>
+      </c>
+      <c r="B21" s="43" t="s">
+        <v>241</v>
+      </c>
+      <c r="C21" s="43" t="s">
+        <v>240</v>
+      </c>
+      <c r="D21" s="43" t="s">
+        <v>0</v>
+      </c>
+      <c r="E21" s="43" t="s">
+        <v>570</v>
+      </c>
+      <c r="F21" s="44" t="s">
+        <v>1552</v>
+      </c>
+      <c r="G21" s="44" t="s">
+        <v>1548</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" s="11" customFormat="1" ht="14">
+      <c r="A22" s="12" t="s">
+        <v>1489</v>
+      </c>
+      <c r="B22" s="12"/>
+      <c r="C22" s="12" t="s">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" s="3" customFormat="1" ht="14">
+      <c r="A23" s="3" t="s">
+        <v>1490</v>
+      </c>
+      <c r="D23" s="3" t="s">
+        <v>1546</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" s="3" customFormat="1" ht="14">
+      <c r="A24" s="3" t="s">
+        <v>1549</v>
+      </c>
+      <c r="E24" s="3" t="s">
+        <v>1545</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" s="3" customFormat="1" ht="28">
+      <c r="A25" s="3" t="s">
+        <v>1491</v>
+      </c>
+      <c r="F25" s="3" t="s">
+        <v>876</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" s="3" customFormat="1" ht="14">
+      <c r="A26" s="3" t="s">
+        <v>1492</v>
+      </c>
+      <c r="G26" s="3" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" s="3" customFormat="1" ht="14" customHeight="1">
+      <c r="A27" s="3" t="s">
+        <v>1493</v>
+      </c>
+      <c r="F27" s="3" t="s">
+        <v>877</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" s="3" customFormat="1" ht="14" customHeight="1">
+      <c r="A28" s="1" t="s">
+        <v>1494</v>
+      </c>
+      <c r="G28" s="3" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" s="3" customFormat="1" ht="14" customHeight="1">
+      <c r="A29" s="3" t="s">
+        <v>1495</v>
+      </c>
+      <c r="F29" s="3" t="s">
+        <v>878</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" s="3" customFormat="1" ht="14" customHeight="1">
+      <c r="A30" s="3" t="s">
+        <v>1496</v>
+      </c>
+      <c r="G30" s="3" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" s="3" customFormat="1" ht="14" customHeight="1">
+      <c r="A31" s="3" t="s">
+        <v>1497</v>
+      </c>
+      <c r="F31" s="3" t="s">
+        <v>879</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" s="3" customFormat="1" ht="14" customHeight="1">
+      <c r="A32" s="3" t="s">
+        <v>1498</v>
+      </c>
+      <c r="G32" s="3" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7" s="3" customFormat="1" ht="14" customHeight="1">
+      <c r="A33" s="3" t="s">
+        <v>1499</v>
+      </c>
+      <c r="F33" s="3" t="s">
+        <v>880</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7" s="3" customFormat="1" ht="14" customHeight="1">
+      <c r="A34" s="3" t="s">
+        <v>1500</v>
+      </c>
+      <c r="G34" s="3" t="s">
+        <v>99</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A1:G1"/>
+  </mergeCells>
+  <phoneticPr fontId="3" type="noConversion"/>
+  <pageMargins left="0.75000000000000011" right="0.75000000000000011" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup scale="65" orientation="landscape" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="100"/>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr enableFormatConditionsCalculation="0">
@@ -8088,32 +8877,32 @@
   <dimension ref="A1:G665"/>
   <sheetViews>
     <sheetView zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A491" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C526" sqref="C526"/>
+      <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" sqref="A1:XFD2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="30.6640625" style="3" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="25.6640625" style="3" customWidth="1"/>
-    <col min="3" max="3" width="52.33203125" style="3" customWidth="1"/>
-    <col min="4" max="4" width="30.5" style="3" customWidth="1"/>
-    <col min="5" max="5" width="30.1640625" style="3" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="41.1640625" style="3" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="21.6640625" style="3" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="46.83203125" style="3" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="17.6640625" style="3" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.33203125" style="3" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="41.33203125" style="3" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="57.83203125" style="3" bestFit="1" customWidth="1"/>
     <col min="8" max="16384" width="10.83203125" style="3"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" customFormat="1" ht="24" customHeight="1">
-      <c r="A1" s="34" t="s">
+      <c r="A1" s="47" t="s">
         <v>269</v>
       </c>
-      <c r="B1" s="34"/>
-      <c r="C1" s="34"/>
-      <c r="D1" s="34"/>
-      <c r="E1" s="34"/>
-      <c r="F1" s="34"/>
-      <c r="G1" s="34"/>
+      <c r="B1" s="47"/>
+      <c r="C1" s="47"/>
+      <c r="D1" s="47"/>
+      <c r="E1" s="47"/>
+      <c r="F1" s="47"/>
+      <c r="G1" s="47"/>
     </row>
     <row r="2" spans="1:7" s="1" customFormat="1" ht="28" customHeight="1">
       <c r="A2" s="1" t="s">
@@ -12213,7 +13002,7 @@
       </c>
     </row>
     <row r="511" spans="1:7">
-      <c r="A511" s="2" t="s">
+      <c r="A511" s="3" t="s">
         <v>1206</v>
       </c>
       <c r="G511" s="3" t="s">
@@ -12278,7 +13067,7 @@
       </c>
     </row>
     <row r="519" spans="1:7">
-      <c r="A519" s="2" t="s">
+      <c r="A519" s="3" t="s">
         <v>1214</v>
       </c>
       <c r="F519" s="3" t="s">
@@ -12647,11 +13436,131 @@
   <sheetPr enableFormatConditionsCalculation="0">
     <tabColor theme="3" tint="0.59999389629810485"/>
   </sheetPr>
-  <dimension ref="A1:E117"/>
+  <dimension ref="A1:E3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F2" sqref="F1:F1048576"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <cols>
+    <col min="3" max="3" width="33.83203125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" ht="24" customHeight="1">
+      <c r="A1" s="47" t="s">
+        <v>269</v>
+      </c>
+      <c r="B1" s="47"/>
+      <c r="C1" s="47"/>
+      <c r="D1" s="47"/>
+      <c r="E1" s="47"/>
+    </row>
+    <row r="2" spans="1:5" s="1" customFormat="1" ht="28" customHeight="1">
+      <c r="A2" s="1" t="s">
+        <v>912</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>241</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>240</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>1556</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>1555</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5">
+      <c r="C3" t="s">
+        <v>1553</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A1:E1"/>
+  </mergeCells>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr enableFormatConditionsCalculation="0">
+    <tabColor theme="3" tint="0.59999389629810485"/>
+  </sheetPr>
+  <dimension ref="A1:E3"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D4" sqref="D4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <cols>
+    <col min="3" max="3" width="36.1640625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" ht="24" customHeight="1">
+      <c r="A1" s="47" t="s">
+        <v>269</v>
+      </c>
+      <c r="B1" s="47"/>
+      <c r="C1" s="47"/>
+      <c r="D1" s="47"/>
+      <c r="E1" s="47"/>
+    </row>
+    <row r="2" spans="1:5" s="1" customFormat="1" ht="28" customHeight="1">
+      <c r="A2" s="1" t="s">
+        <v>912</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>241</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>240</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>1556</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>1555</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5">
+      <c r="C3" t="s">
+        <v>1554</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A1:E1"/>
+  </mergeCells>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr enableFormatConditionsCalculation="0">
+    <tabColor theme="3" tint="0.59999389629810485"/>
+  </sheetPr>
+  <dimension ref="A1:E116"/>
   <sheetViews>
     <sheetView zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A57" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C135" sqref="C135"/>
+      <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14" x14ac:dyDescent="0"/>
@@ -12665,13 +13574,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" customFormat="1" ht="24" customHeight="1">
-      <c r="A1" s="34" t="s">
+      <c r="A1" s="47" t="s">
         <v>269</v>
       </c>
-      <c r="B1" s="34"/>
-      <c r="C1" s="34"/>
-      <c r="D1" s="34"/>
-      <c r="E1" s="34"/>
+      <c r="B1" s="47"/>
+      <c r="C1" s="47"/>
+      <c r="D1" s="47"/>
+      <c r="E1" s="47"/>
     </row>
     <row r="2" spans="1:5" s="1" customFormat="1" ht="28" customHeight="1">
       <c r="A2" s="1" t="s">
@@ -12690,913 +13599,908 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:5" s="2" customFormat="1">
-      <c r="A3" s="2" t="s">
-        <v>1420</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" s="11" customFormat="1">
-      <c r="A4" s="11" t="s">
+    <row r="3" spans="1:5" s="11" customFormat="1">
+      <c r="A3" s="11" t="s">
         <v>1421</v>
       </c>
-      <c r="B4" s="12"/>
-      <c r="C4" s="12" t="s">
+      <c r="B3" s="12"/>
+      <c r="C3" s="12" t="s">
         <v>252</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5">
+      <c r="A4" s="3" t="s">
+        <v>1422</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>385</v>
       </c>
     </row>
     <row r="5" spans="1:5">
       <c r="A5" s="3" t="s">
-        <v>1422</v>
-      </c>
-      <c r="D5" s="3" t="s">
-        <v>385</v>
+        <v>1423</v>
+      </c>
+      <c r="E5" s="3" t="s">
+        <v>99</v>
       </c>
     </row>
     <row r="6" spans="1:5">
       <c r="A6" s="3" t="s">
-        <v>1423</v>
-      </c>
-      <c r="E6" s="3" t="s">
-        <v>99</v>
+        <v>1424</v>
+      </c>
+      <c r="D6" s="3" t="s">
+        <v>386</v>
       </c>
     </row>
     <row r="7" spans="1:5">
       <c r="A7" s="3" t="s">
-        <v>1424</v>
-      </c>
-      <c r="D7" s="3" t="s">
-        <v>386</v>
+        <v>1425</v>
+      </c>
+      <c r="E7" s="3" t="s">
+        <v>387</v>
       </c>
     </row>
     <row r="8" spans="1:5">
       <c r="A8" s="3" t="s">
-        <v>1425</v>
+        <v>1426</v>
       </c>
       <c r="E8" s="3" t="s">
-        <v>387</v>
+        <v>388</v>
       </c>
     </row>
     <row r="9" spans="1:5">
       <c r="A9" s="3" t="s">
-        <v>1426</v>
+        <v>1427</v>
       </c>
       <c r="E9" s="3" t="s">
-        <v>388</v>
+        <v>389</v>
       </c>
     </row>
     <row r="10" spans="1:5">
       <c r="A10" s="3" t="s">
-        <v>1427</v>
-      </c>
-      <c r="E10" s="3" t="s">
-        <v>389</v>
+        <v>1428</v>
+      </c>
+      <c r="D10" s="3" t="s">
+        <v>390</v>
       </c>
     </row>
     <row r="11" spans="1:5">
       <c r="A11" s="3" t="s">
-        <v>1428</v>
-      </c>
-      <c r="D11" s="3" t="s">
-        <v>390</v>
+        <v>1429</v>
+      </c>
+      <c r="E11" s="3" t="s">
+        <v>99</v>
       </c>
     </row>
     <row r="12" spans="1:5">
       <c r="A12" s="3" t="s">
-        <v>1429</v>
-      </c>
-      <c r="E12" s="3" t="s">
-        <v>99</v>
+        <v>1430</v>
+      </c>
+      <c r="D12" s="3" t="s">
+        <v>391</v>
       </c>
     </row>
     <row r="13" spans="1:5">
       <c r="A13" s="3" t="s">
-        <v>1430</v>
-      </c>
-      <c r="D13" s="3" t="s">
-        <v>391</v>
+        <v>1431</v>
+      </c>
+      <c r="E13" s="3" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="14" spans="1:5">
       <c r="A14" s="3" t="s">
-        <v>1431</v>
-      </c>
-      <c r="E14" s="3" t="s">
-        <v>7</v>
+        <v>1432</v>
+      </c>
+      <c r="D14" s="3" t="s">
+        <v>392</v>
       </c>
     </row>
     <row r="15" spans="1:5">
       <c r="A15" s="3" t="s">
-        <v>1432</v>
-      </c>
-      <c r="D15" s="3" t="s">
-        <v>392</v>
+        <v>1433</v>
+      </c>
+      <c r="E15" s="3" t="s">
+        <v>393</v>
       </c>
     </row>
     <row r="16" spans="1:5">
       <c r="A16" s="3" t="s">
-        <v>1433</v>
+        <v>1434</v>
       </c>
       <c r="E16" s="3" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
     </row>
     <row r="17" spans="1:5">
       <c r="A17" s="3" t="s">
-        <v>1434</v>
+        <v>1435</v>
       </c>
       <c r="E17" s="3" t="s">
-        <v>394</v>
+        <v>395</v>
       </c>
     </row>
     <row r="18" spans="1:5">
       <c r="A18" s="3" t="s">
-        <v>1435</v>
+        <v>1436</v>
       </c>
       <c r="E18" s="3" t="s">
-        <v>395</v>
+        <v>396</v>
       </c>
     </row>
     <row r="19" spans="1:5">
       <c r="A19" s="3" t="s">
-        <v>1436</v>
+        <v>1437</v>
       </c>
       <c r="E19" s="3" t="s">
-        <v>396</v>
+        <v>397</v>
       </c>
     </row>
     <row r="20" spans="1:5">
       <c r="A20" s="3" t="s">
-        <v>1437</v>
-      </c>
-      <c r="E20" s="3" t="s">
-        <v>397</v>
+        <v>1438</v>
+      </c>
+      <c r="D20" s="3" t="s">
+        <v>398</v>
       </c>
     </row>
     <row r="21" spans="1:5">
       <c r="A21" s="3" t="s">
-        <v>1438</v>
-      </c>
-      <c r="D21" s="3" t="s">
-        <v>398</v>
+        <v>1439</v>
+      </c>
+      <c r="E21" s="3" t="s">
+        <v>399</v>
       </c>
     </row>
     <row r="22" spans="1:5">
       <c r="A22" s="3" t="s">
-        <v>1439</v>
+        <v>1440</v>
       </c>
       <c r="E22" s="3" t="s">
-        <v>399</v>
+        <v>400</v>
       </c>
     </row>
     <row r="23" spans="1:5">
       <c r="A23" s="3" t="s">
-        <v>1440</v>
+        <v>1441</v>
       </c>
       <c r="E23" s="3" t="s">
-        <v>400</v>
+        <v>401</v>
       </c>
     </row>
     <row r="24" spans="1:5">
       <c r="A24" s="3" t="s">
-        <v>1441</v>
+        <v>1442</v>
       </c>
       <c r="E24" s="3" t="s">
-        <v>401</v>
+        <v>29</v>
       </c>
     </row>
     <row r="25" spans="1:5">
       <c r="A25" s="3" t="s">
-        <v>1442</v>
+        <v>1443</v>
       </c>
       <c r="E25" s="3" t="s">
-        <v>29</v>
+        <v>402</v>
       </c>
     </row>
     <row r="26" spans="1:5">
       <c r="A26" s="3" t="s">
-        <v>1443</v>
-      </c>
-      <c r="E26" s="3" t="s">
-        <v>402</v>
+        <v>1444</v>
+      </c>
+      <c r="D26" s="3" t="s">
+        <v>403</v>
       </c>
     </row>
     <row r="27" spans="1:5">
       <c r="A27" s="3" t="s">
-        <v>1444</v>
-      </c>
-      <c r="D27" s="3" t="s">
-        <v>403</v>
+        <v>1445</v>
+      </c>
+      <c r="E27" s="3" t="s">
+        <v>404</v>
       </c>
     </row>
     <row r="28" spans="1:5">
       <c r="A28" s="3" t="s">
-        <v>1445</v>
+        <v>1446</v>
       </c>
       <c r="E28" s="3" t="s">
-        <v>404</v>
+        <v>21</v>
       </c>
     </row>
     <row r="29" spans="1:5">
       <c r="A29" s="3" t="s">
-        <v>1446</v>
+        <v>1447</v>
       </c>
       <c r="E29" s="3" t="s">
-        <v>21</v>
+        <v>405</v>
       </c>
     </row>
     <row r="30" spans="1:5">
       <c r="A30" s="3" t="s">
-        <v>1447</v>
+        <v>1448</v>
       </c>
       <c r="E30" s="3" t="s">
-        <v>405</v>
+        <v>183</v>
       </c>
     </row>
     <row r="31" spans="1:5">
       <c r="A31" s="3" t="s">
-        <v>1448</v>
+        <v>1449</v>
       </c>
       <c r="E31" s="3" t="s">
-        <v>183</v>
+        <v>29</v>
       </c>
     </row>
     <row r="32" spans="1:5">
       <c r="A32" s="3" t="s">
-        <v>1449</v>
-      </c>
-      <c r="E32" s="3" t="s">
-        <v>29</v>
+        <v>1450</v>
+      </c>
+      <c r="D32" s="3" t="s">
+        <v>406</v>
       </c>
     </row>
     <row r="33" spans="1:5">
       <c r="A33" s="3" t="s">
-        <v>1450</v>
-      </c>
-      <c r="D33" s="3" t="s">
-        <v>406</v>
+        <v>1451</v>
+      </c>
+      <c r="E33" s="3" t="s">
+        <v>407</v>
       </c>
     </row>
     <row r="34" spans="1:5">
       <c r="A34" s="3" t="s">
-        <v>1451</v>
+        <v>1452</v>
       </c>
       <c r="E34" s="3" t="s">
-        <v>407</v>
+        <v>408</v>
       </c>
     </row>
     <row r="35" spans="1:5">
       <c r="A35" s="3" t="s">
-        <v>1452</v>
+        <v>1453</v>
       </c>
       <c r="E35" s="3" t="s">
-        <v>408</v>
+        <v>409</v>
       </c>
     </row>
     <row r="36" spans="1:5">
       <c r="A36" s="3" t="s">
-        <v>1453</v>
-      </c>
-      <c r="E36" s="3" t="s">
-        <v>409</v>
+        <v>1454</v>
+      </c>
+      <c r="D36" s="3" t="s">
+        <v>410</v>
       </c>
     </row>
     <row r="37" spans="1:5">
       <c r="A37" s="3" t="s">
-        <v>1454</v>
-      </c>
-      <c r="D37" s="3" t="s">
-        <v>410</v>
+        <v>1455</v>
+      </c>
+      <c r="E37" s="3" t="s">
+        <v>407</v>
       </c>
     </row>
     <row r="38" spans="1:5">
       <c r="A38" s="3" t="s">
-        <v>1455</v>
+        <v>1456</v>
       </c>
       <c r="E38" s="3" t="s">
-        <v>407</v>
+        <v>411</v>
       </c>
     </row>
     <row r="39" spans="1:5">
       <c r="A39" s="3" t="s">
-        <v>1456</v>
+        <v>1457</v>
       </c>
       <c r="E39" s="3" t="s">
-        <v>411</v>
-      </c>
-    </row>
-    <row r="40" spans="1:5">
+        <v>412</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5" s="11" customFormat="1">
       <c r="A40" s="3" t="s">
-        <v>1457</v>
-      </c>
-      <c r="E40" s="3" t="s">
-        <v>412</v>
-      </c>
-    </row>
-    <row r="41" spans="1:5" s="11" customFormat="1">
+        <v>1458</v>
+      </c>
+      <c r="B40" s="12"/>
+      <c r="C40" s="12" t="s">
+        <v>886</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5" s="2" customFormat="1">
       <c r="A41" s="3" t="s">
-        <v>1458</v>
-      </c>
-      <c r="B41" s="12"/>
-      <c r="C41" s="12" t="s">
-        <v>886</v>
-      </c>
-    </row>
-    <row r="42" spans="1:5" s="2" customFormat="1">
+        <v>1459</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5" customFormat="1" ht="15">
       <c r="A42" s="3" t="s">
-        <v>1459</v>
-      </c>
+        <v>1460</v>
+      </c>
+      <c r="D42" s="6" t="s">
+        <v>413</v>
+      </c>
+      <c r="E42" s="3"/>
     </row>
     <row r="43" spans="1:5" customFormat="1" ht="15">
       <c r="A43" s="3" t="s">
-        <v>1460</v>
-      </c>
-      <c r="D43" s="6" t="s">
-        <v>413</v>
-      </c>
-      <c r="E43" s="3"/>
-    </row>
-    <row r="44" spans="1:5" customFormat="1" ht="15">
+        <v>1461</v>
+      </c>
+      <c r="D43" s="6"/>
+      <c r="E43" s="3" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5">
       <c r="A44" s="3" t="s">
-        <v>1461</v>
-      </c>
-      <c r="D44" s="6"/>
-      <c r="E44" s="3" t="s">
+        <v>1462</v>
+      </c>
+      <c r="D44" s="3" t="s">
+        <v>414</v>
+      </c>
+    </row>
+    <row r="45" spans="1:5">
+      <c r="A45" s="11" t="s">
+        <v>1463</v>
+      </c>
+      <c r="E45" s="3" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="45" spans="1:5">
-      <c r="A45" s="3" t="s">
-        <v>1462</v>
-      </c>
-      <c r="D45" s="3" t="s">
-        <v>414</v>
-      </c>
-    </row>
     <row r="46" spans="1:5">
-      <c r="A46" s="11" t="s">
-        <v>1463</v>
-      </c>
-      <c r="E46" s="3" t="s">
-        <v>99</v>
+      <c r="A46" s="2" t="s">
+        <v>1464</v>
+      </c>
+      <c r="D46" s="3" t="s">
+        <v>415</v>
       </c>
     </row>
     <row r="47" spans="1:5">
       <c r="A47" s="2" t="s">
-        <v>1464</v>
-      </c>
-      <c r="D47" s="3" t="s">
-        <v>415</v>
+        <v>1465</v>
+      </c>
+      <c r="E47" s="3" t="s">
+        <v>99</v>
       </c>
     </row>
     <row r="48" spans="1:5">
       <c r="A48" s="2" t="s">
-        <v>1465</v>
-      </c>
-      <c r="E48" s="3" t="s">
+        <v>1466</v>
+      </c>
+      <c r="D48" s="3" t="s">
+        <v>416</v>
+      </c>
+    </row>
+    <row r="49" spans="1:5">
+      <c r="A49" s="3" t="s">
+        <v>1467</v>
+      </c>
+      <c r="E49" s="3" t="s">
         <v>99</v>
-      </c>
-    </row>
-    <row r="49" spans="1:5">
-      <c r="A49" s="2" t="s">
-        <v>1466</v>
-      </c>
-      <c r="D49" s="3" t="s">
-        <v>416</v>
       </c>
     </row>
     <row r="50" spans="1:5">
       <c r="A50" s="3" t="s">
-        <v>1467</v>
-      </c>
-      <c r="E50" s="3" t="s">
-        <v>99</v>
+        <v>1468</v>
+      </c>
+      <c r="D50" s="3" t="s">
+        <v>417</v>
       </c>
     </row>
     <row r="51" spans="1:5">
       <c r="A51" s="3" t="s">
-        <v>1468</v>
-      </c>
-      <c r="D51" s="3" t="s">
-        <v>417</v>
+        <v>1469</v>
+      </c>
+      <c r="E51" s="3" t="s">
+        <v>99</v>
       </c>
     </row>
     <row r="52" spans="1:5">
       <c r="A52" s="3" t="s">
-        <v>1469</v>
-      </c>
-      <c r="E52" s="3" t="s">
-        <v>99</v>
+        <v>1470</v>
+      </c>
+      <c r="D52" s="3" t="s">
+        <v>418</v>
       </c>
     </row>
     <row r="53" spans="1:5">
       <c r="A53" s="3" t="s">
-        <v>1470</v>
-      </c>
-      <c r="D53" s="3" t="s">
-        <v>418</v>
+        <v>1471</v>
+      </c>
+      <c r="E53" s="3" t="s">
+        <v>99</v>
       </c>
     </row>
     <row r="54" spans="1:5">
       <c r="A54" s="3" t="s">
-        <v>1471</v>
-      </c>
-      <c r="E54" s="3" t="s">
-        <v>99</v>
+        <v>1472</v>
+      </c>
+      <c r="D54" s="3" t="s">
+        <v>419</v>
       </c>
     </row>
     <row r="55" spans="1:5">
       <c r="A55" s="3" t="s">
-        <v>1472</v>
-      </c>
-      <c r="D55" s="3" t="s">
-        <v>419</v>
+        <v>1473</v>
+      </c>
+      <c r="E55" s="3" t="s">
+        <v>420</v>
       </c>
     </row>
     <row r="56" spans="1:5">
       <c r="A56" s="3" t="s">
-        <v>1473</v>
+        <v>1474</v>
       </c>
       <c r="E56" s="3" t="s">
-        <v>420</v>
+        <v>421</v>
       </c>
     </row>
     <row r="57" spans="1:5">
       <c r="A57" s="3" t="s">
-        <v>1474</v>
-      </c>
-      <c r="E57" s="3" t="s">
-        <v>421</v>
+        <v>1475</v>
+      </c>
+      <c r="D57" s="3" t="s">
+        <v>422</v>
       </c>
     </row>
     <row r="58" spans="1:5">
       <c r="A58" s="3" t="s">
-        <v>1475</v>
-      </c>
-      <c r="D58" s="3" t="s">
-        <v>422</v>
+        <v>1476</v>
+      </c>
+      <c r="E58" s="3" t="s">
+        <v>423</v>
       </c>
     </row>
     <row r="59" spans="1:5">
       <c r="A59" s="3" t="s">
-        <v>1476</v>
-      </c>
-      <c r="E59" s="3" t="s">
-        <v>423</v>
+        <v>1477</v>
+      </c>
+      <c r="E59" s="4" t="s">
+        <v>887</v>
       </c>
     </row>
     <row r="60" spans="1:5">
       <c r="A60" s="3" t="s">
-        <v>1477</v>
-      </c>
-      <c r="E60" s="4" t="s">
-        <v>887</v>
+        <v>1478</v>
+      </c>
+      <c r="E60" s="3" t="s">
+        <v>424</v>
       </c>
     </row>
     <row r="61" spans="1:5">
       <c r="A61" s="3" t="s">
-        <v>1478</v>
+        <v>1479</v>
       </c>
       <c r="E61" s="3" t="s">
-        <v>424</v>
+        <v>425</v>
       </c>
     </row>
     <row r="62" spans="1:5">
       <c r="A62" s="3" t="s">
-        <v>1479</v>
+        <v>1480</v>
       </c>
       <c r="E62" s="3" t="s">
-        <v>425</v>
+        <v>426</v>
       </c>
     </row>
     <row r="63" spans="1:5">
       <c r="A63" s="3" t="s">
-        <v>1480</v>
+        <v>1481</v>
       </c>
       <c r="E63" s="3" t="s">
-        <v>426</v>
+        <v>427</v>
       </c>
     </row>
     <row r="64" spans="1:5">
       <c r="A64" s="3" t="s">
-        <v>1481</v>
+        <v>1482</v>
       </c>
       <c r="E64" s="3" t="s">
-        <v>427</v>
+        <v>428</v>
       </c>
     </row>
     <row r="65" spans="1:5">
       <c r="A65" s="3" t="s">
-        <v>1482</v>
-      </c>
-      <c r="E65" s="3" t="s">
-        <v>428</v>
+        <v>1483</v>
+      </c>
+      <c r="D65" s="3" t="s">
+        <v>429</v>
       </c>
     </row>
     <row r="66" spans="1:5">
       <c r="A66" s="3" t="s">
-        <v>1483</v>
-      </c>
-      <c r="D66" s="3" t="s">
-        <v>429</v>
+        <v>1484</v>
+      </c>
+      <c r="E66" s="3" t="s">
+        <v>99</v>
       </c>
     </row>
     <row r="67" spans="1:5">
       <c r="A67" s="3" t="s">
-        <v>1484</v>
-      </c>
-      <c r="E67" s="3" t="s">
-        <v>99</v>
+        <v>1485</v>
+      </c>
+      <c r="D67" s="3" t="s">
+        <v>430</v>
       </c>
     </row>
     <row r="68" spans="1:5">
       <c r="A68" s="3" t="s">
-        <v>1485</v>
-      </c>
-      <c r="D68" s="3" t="s">
-        <v>430</v>
+        <v>1486</v>
+      </c>
+      <c r="E68" s="3" t="s">
+        <v>99</v>
       </c>
     </row>
     <row r="69" spans="1:5">
       <c r="A69" s="3" t="s">
-        <v>1486</v>
-      </c>
-      <c r="E69" s="3" t="s">
-        <v>99</v>
+        <v>1487</v>
+      </c>
+      <c r="D69" s="3" t="s">
+        <v>431</v>
       </c>
     </row>
     <row r="70" spans="1:5">
       <c r="A70" s="3" t="s">
-        <v>1487</v>
-      </c>
-      <c r="D70" s="3" t="s">
-        <v>431</v>
-      </c>
-    </row>
-    <row r="71" spans="1:5">
+        <v>1488</v>
+      </c>
+      <c r="E70" s="3" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="71" spans="1:5" s="11" customFormat="1">
       <c r="A71" s="3" t="s">
-        <v>1488</v>
-      </c>
-      <c r="E71" s="3" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="72" spans="1:5" s="11" customFormat="1">
+        <v>1489</v>
+      </c>
+      <c r="B71" s="12"/>
+      <c r="C71" s="12" t="s">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="72" spans="1:5">
       <c r="A72" s="3" t="s">
-        <v>1489</v>
-      </c>
-      <c r="B72" s="12"/>
-      <c r="C72" s="12" t="s">
-        <v>253</v>
+        <v>1490</v>
       </c>
     </row>
     <row r="73" spans="1:5">
       <c r="A73" s="3" t="s">
-        <v>1490</v>
+        <v>1491</v>
+      </c>
+      <c r="D73" s="3" t="s">
+        <v>876</v>
       </c>
     </row>
     <row r="74" spans="1:5">
       <c r="A74" s="3" t="s">
-        <v>1491</v>
-      </c>
-      <c r="D74" s="3" t="s">
-        <v>876</v>
-      </c>
-    </row>
-    <row r="75" spans="1:5">
+        <v>1492</v>
+      </c>
+      <c r="E74" s="3" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="75" spans="1:5" ht="14" customHeight="1">
       <c r="A75" s="3" t="s">
-        <v>1492</v>
-      </c>
-      <c r="E75" s="3" t="s">
+        <v>1493</v>
+      </c>
+      <c r="D75" s="3" t="s">
+        <v>877</v>
+      </c>
+    </row>
+    <row r="76" spans="1:5" ht="14" customHeight="1">
+      <c r="A76" s="11" t="s">
+        <v>1494</v>
+      </c>
+      <c r="E76" s="3" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="76" spans="1:5" ht="14" customHeight="1">
-      <c r="A76" s="3" t="s">
-        <v>1493</v>
-      </c>
-      <c r="D76" s="3" t="s">
-        <v>877</v>
-      </c>
-    </row>
     <row r="77" spans="1:5" ht="14" customHeight="1">
-      <c r="A77" s="11" t="s">
-        <v>1494</v>
-      </c>
-      <c r="E77" s="3" t="s">
-        <v>99</v>
+      <c r="A77" s="3" t="s">
+        <v>1495</v>
+      </c>
+      <c r="D77" s="3" t="s">
+        <v>878</v>
       </c>
     </row>
     <row r="78" spans="1:5" ht="14" customHeight="1">
       <c r="A78" s="3" t="s">
-        <v>1495</v>
-      </c>
-      <c r="D78" s="3" t="s">
-        <v>878</v>
+        <v>1496</v>
+      </c>
+      <c r="E78" s="3" t="s">
+        <v>99</v>
       </c>
     </row>
     <row r="79" spans="1:5" ht="14" customHeight="1">
       <c r="A79" s="3" t="s">
-        <v>1496</v>
-      </c>
-      <c r="E79" s="3" t="s">
-        <v>99</v>
+        <v>1497</v>
+      </c>
+      <c r="D79" s="3" t="s">
+        <v>879</v>
       </c>
     </row>
     <row r="80" spans="1:5" ht="14" customHeight="1">
       <c r="A80" s="3" t="s">
-        <v>1497</v>
-      </c>
-      <c r="D80" s="3" t="s">
-        <v>879</v>
+        <v>1498</v>
+      </c>
+      <c r="E80" s="3" t="s">
+        <v>99</v>
       </c>
     </row>
     <row r="81" spans="1:5" ht="14" customHeight="1">
       <c r="A81" s="3" t="s">
-        <v>1498</v>
-      </c>
-      <c r="E81" s="3" t="s">
-        <v>99</v>
+        <v>1499</v>
+      </c>
+      <c r="D81" s="3" t="s">
+        <v>880</v>
       </c>
     </row>
     <row r="82" spans="1:5" ht="14" customHeight="1">
       <c r="A82" s="3" t="s">
-        <v>1499</v>
-      </c>
-      <c r="D82" s="3" t="s">
-        <v>880</v>
+        <v>1500</v>
+      </c>
+      <c r="E82" s="3" t="s">
+        <v>99</v>
       </c>
     </row>
     <row r="83" spans="1:5" ht="14" customHeight="1">
       <c r="A83" s="3" t="s">
-        <v>1500</v>
-      </c>
-      <c r="E83" s="3" t="s">
-        <v>99</v>
+        <v>1501</v>
       </c>
     </row>
     <row r="84" spans="1:5" ht="14" customHeight="1">
       <c r="A84" s="3" t="s">
-        <v>1501</v>
+        <v>1502</v>
+      </c>
+      <c r="D84" s="3" t="s">
+        <v>434</v>
       </c>
     </row>
     <row r="85" spans="1:5" ht="14" customHeight="1">
       <c r="A85" s="3" t="s">
-        <v>1502</v>
-      </c>
-      <c r="D85" s="3" t="s">
-        <v>434</v>
-      </c>
-    </row>
-    <row r="86" spans="1:5" ht="14" customHeight="1">
+        <v>1503</v>
+      </c>
+      <c r="E85" s="3" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="86" spans="1:5">
       <c r="A86" s="3" t="s">
-        <v>1503</v>
-      </c>
-      <c r="E86" s="3" t="s">
-        <v>99</v>
+        <v>1504</v>
+      </c>
+      <c r="D86" s="3" t="s">
+        <v>435</v>
       </c>
     </row>
     <row r="87" spans="1:5">
       <c r="A87" s="3" t="s">
-        <v>1504</v>
-      </c>
-      <c r="D87" s="3" t="s">
-        <v>435</v>
-      </c>
-    </row>
-    <row r="88" spans="1:5">
+        <v>1505</v>
+      </c>
+      <c r="E87" s="3" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="88" spans="1:5" ht="16" customHeight="1">
       <c r="A88" s="3" t="s">
-        <v>1505</v>
-      </c>
-      <c r="E88" s="3" t="s">
-        <v>99</v>
+        <v>1506</v>
+      </c>
+      <c r="D88" s="3" t="s">
+        <v>436</v>
       </c>
     </row>
     <row r="89" spans="1:5" ht="16" customHeight="1">
       <c r="A89" s="3" t="s">
-        <v>1506</v>
-      </c>
-      <c r="D89" s="3" t="s">
-        <v>436</v>
-      </c>
-    </row>
-    <row r="90" spans="1:5" ht="16" customHeight="1">
+        <v>1507</v>
+      </c>
+      <c r="E89" s="3" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="90" spans="1:5">
       <c r="A90" s="3" t="s">
-        <v>1507</v>
-      </c>
-      <c r="E90" s="3" t="s">
-        <v>99</v>
+        <v>1508</v>
+      </c>
+      <c r="D90" s="3" t="s">
+        <v>881</v>
       </c>
     </row>
     <row r="91" spans="1:5">
       <c r="A91" s="3" t="s">
-        <v>1508</v>
-      </c>
-      <c r="D91" s="3" t="s">
-        <v>881</v>
-      </c>
-    </row>
-    <row r="92" spans="1:5">
+        <v>1509</v>
+      </c>
+      <c r="E91" s="3" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="92" spans="1:5" ht="28">
       <c r="A92" s="3" t="s">
-        <v>1509</v>
-      </c>
-      <c r="E92" s="3" t="s">
+        <v>1510</v>
+      </c>
+      <c r="D92" s="3" t="s">
+        <v>882</v>
+      </c>
+    </row>
+    <row r="93" spans="1:5">
+      <c r="A93" s="3" t="s">
+        <v>1511</v>
+      </c>
+      <c r="E93" s="4" t="s">
         <v>99</v>
-      </c>
-    </row>
-    <row r="93" spans="1:5" ht="28">
-      <c r="A93" s="3" t="s">
-        <v>1510</v>
-      </c>
-      <c r="D93" s="3" t="s">
-        <v>882</v>
       </c>
     </row>
     <row r="94" spans="1:5">
       <c r="A94" s="3" t="s">
-        <v>1511</v>
-      </c>
-      <c r="E94" s="4" t="s">
-        <v>99</v>
+        <v>1512</v>
       </c>
     </row>
     <row r="95" spans="1:5">
       <c r="A95" s="3" t="s">
-        <v>1512</v>
+        <v>1513</v>
+      </c>
+      <c r="D95" s="3" t="s">
+        <v>433</v>
       </c>
     </row>
     <row r="96" spans="1:5">
       <c r="A96" s="3" t="s">
-        <v>1513</v>
-      </c>
-      <c r="D96" s="3" t="s">
-        <v>433</v>
+        <v>1514</v>
+      </c>
+      <c r="E96" s="3" t="s">
+        <v>99</v>
       </c>
     </row>
     <row r="97" spans="1:5">
       <c r="A97" s="3" t="s">
-        <v>1514</v>
-      </c>
-      <c r="E97" s="3" t="s">
-        <v>99</v>
+        <v>1515</v>
+      </c>
+      <c r="D97" s="3" t="s">
+        <v>866</v>
       </c>
     </row>
     <row r="98" spans="1:5">
       <c r="A98" s="3" t="s">
-        <v>1515</v>
-      </c>
-      <c r="D98" s="3" t="s">
-        <v>866</v>
+        <v>1516</v>
+      </c>
+      <c r="E98" s="4" t="s">
+        <v>99</v>
       </c>
     </row>
     <row r="99" spans="1:5">
       <c r="A99" s="3" t="s">
-        <v>1516</v>
-      </c>
-      <c r="E99" s="4" t="s">
-        <v>99</v>
+        <v>1517</v>
+      </c>
+      <c r="D99" s="3" t="s">
+        <v>867</v>
       </c>
     </row>
     <row r="100" spans="1:5">
       <c r="A100" s="3" t="s">
-        <v>1517</v>
-      </c>
-      <c r="D100" s="3" t="s">
-        <v>867</v>
+        <v>1518</v>
+      </c>
+      <c r="E100" s="4" t="s">
+        <v>99</v>
       </c>
     </row>
     <row r="101" spans="1:5">
       <c r="A101" s="3" t="s">
-        <v>1518</v>
-      </c>
-      <c r="E101" s="4" t="s">
-        <v>99</v>
+        <v>1519</v>
+      </c>
+      <c r="D101" s="3" t="s">
+        <v>868</v>
       </c>
     </row>
     <row r="102" spans="1:5">
       <c r="A102" s="3" t="s">
-        <v>1519</v>
-      </c>
-      <c r="D102" s="3" t="s">
-        <v>868</v>
+        <v>1520</v>
+      </c>
+      <c r="E102" s="4" t="s">
+        <v>99</v>
       </c>
     </row>
     <row r="103" spans="1:5">
       <c r="A103" s="3" t="s">
-        <v>1520</v>
-      </c>
-      <c r="E103" s="4" t="s">
-        <v>99</v>
+        <v>1521</v>
+      </c>
+      <c r="D103" s="3" t="s">
+        <v>869</v>
       </c>
     </row>
     <row r="104" spans="1:5">
       <c r="A104" s="3" t="s">
-        <v>1521</v>
-      </c>
-      <c r="D104" s="3" t="s">
-        <v>869</v>
+        <v>1522</v>
+      </c>
+      <c r="E104" s="4" t="s">
+        <v>99</v>
       </c>
     </row>
     <row r="105" spans="1:5">
       <c r="A105" s="3" t="s">
-        <v>1522</v>
-      </c>
-      <c r="E105" s="4" t="s">
-        <v>99</v>
+        <v>1523</v>
+      </c>
+      <c r="D105" s="3" t="s">
+        <v>870</v>
       </c>
     </row>
     <row r="106" spans="1:5">
       <c r="A106" s="3" t="s">
-        <v>1523</v>
-      </c>
-      <c r="D106" s="3" t="s">
-        <v>870</v>
+        <v>1524</v>
+      </c>
+      <c r="E106" s="4" t="s">
+        <v>99</v>
       </c>
     </row>
     <row r="107" spans="1:5">
       <c r="A107" s="3" t="s">
-        <v>1524</v>
-      </c>
-      <c r="E107" s="4" t="s">
-        <v>99</v>
+        <v>1525</v>
+      </c>
+      <c r="D107" s="3" t="s">
+        <v>871</v>
       </c>
     </row>
     <row r="108" spans="1:5">
       <c r="A108" s="3" t="s">
-        <v>1525</v>
-      </c>
-      <c r="D108" s="3" t="s">
-        <v>871</v>
+        <v>1526</v>
+      </c>
+      <c r="E108" s="4" t="s">
+        <v>99</v>
       </c>
     </row>
     <row r="109" spans="1:5">
       <c r="A109" s="3" t="s">
-        <v>1526</v>
-      </c>
-      <c r="E109" s="4" t="s">
-        <v>99</v>
+        <v>1527</v>
+      </c>
+      <c r="D109" s="3" t="s">
+        <v>872</v>
       </c>
     </row>
     <row r="110" spans="1:5">
       <c r="A110" s="3" t="s">
-        <v>1527</v>
-      </c>
-      <c r="D110" s="3" t="s">
-        <v>872</v>
+        <v>1528</v>
+      </c>
+      <c r="E110" s="4" t="s">
+        <v>99</v>
       </c>
     </row>
     <row r="111" spans="1:5">
       <c r="A111" s="3" t="s">
-        <v>1528</v>
-      </c>
-      <c r="E111" s="4" t="s">
-        <v>99</v>
+        <v>1529</v>
+      </c>
+      <c r="D111" s="3" t="s">
+        <v>873</v>
       </c>
     </row>
     <row r="112" spans="1:5">
       <c r="A112" s="3" t="s">
-        <v>1529</v>
-      </c>
-      <c r="D112" s="3" t="s">
-        <v>873</v>
+        <v>1530</v>
+      </c>
+      <c r="E112" s="4" t="s">
+        <v>99</v>
       </c>
     </row>
     <row r="113" spans="1:5">
       <c r="A113" s="3" t="s">
-        <v>1530</v>
-      </c>
-      <c r="E113" s="4" t="s">
-        <v>99</v>
+        <v>1531</v>
+      </c>
+      <c r="D113" s="3" t="s">
+        <v>874</v>
       </c>
     </row>
     <row r="114" spans="1:5">
       <c r="A114" s="3" t="s">
-        <v>1531</v>
-      </c>
-      <c r="D114" s="3" t="s">
-        <v>874</v>
+        <v>1532</v>
+      </c>
+      <c r="E114" s="4" t="s">
+        <v>99</v>
       </c>
     </row>
     <row r="115" spans="1:5">
       <c r="A115" s="3" t="s">
-        <v>1532</v>
-      </c>
-      <c r="E115" s="4" t="s">
-        <v>99</v>
+        <v>1533</v>
+      </c>
+      <c r="D115" s="3" t="s">
+        <v>875</v>
       </c>
     </row>
     <row r="116" spans="1:5">
       <c r="A116" s="3" t="s">
-        <v>1533</v>
-      </c>
-      <c r="D116" s="3" t="s">
-        <v>875</v>
-      </c>
-    </row>
-    <row r="117" spans="1:5">
-      <c r="A117" s="3" t="s">
         <v>1534</v>
       </c>
-      <c r="E117" s="4" t="s">
+      <c r="E116" s="4" t="s">
         <v>99</v>
       </c>
     </row>
@@ -13615,16 +14519,16 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr enableFormatConditionsCalculation="0">
     <tabColor theme="3" tint="0.59999389629810485"/>
   </sheetPr>
   <dimension ref="A1:G50"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
+    <sheetView zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F3" sqref="F3"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2:XFD15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14" x14ac:dyDescent="0"/>
@@ -13641,15 +14545,15 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" customFormat="1" ht="24" customHeight="1">
-      <c r="A1" s="34" t="s">
+      <c r="A1" s="47" t="s">
         <v>269</v>
       </c>
-      <c r="B1" s="34"/>
-      <c r="C1" s="34"/>
-      <c r="D1" s="34"/>
-      <c r="E1" s="34"/>
-      <c r="F1" s="34"/>
-      <c r="G1" s="34"/>
+      <c r="B1" s="47"/>
+      <c r="C1" s="47"/>
+      <c r="D1" s="47"/>
+      <c r="E1" s="47"/>
+      <c r="F1" s="47"/>
+      <c r="G1" s="47"/>
     </row>
     <row r="2" spans="1:7" s="1" customFormat="1" ht="28" customHeight="1">
       <c r="A2" s="1" t="s">
@@ -14074,7 +14978,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr enableFormatConditionsCalculation="0">
     <tabColor theme="9" tint="0.39997558519241921"/>
@@ -14099,14 +15003,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="24" customHeight="1">
-      <c r="A1" s="35" t="s">
+      <c r="A1" s="48" t="s">
         <v>262</v>
       </c>
-      <c r="B1" s="35"/>
-      <c r="C1" s="35"/>
-      <c r="D1" s="35"/>
-      <c r="E1" s="35"/>
-      <c r="F1" s="35"/>
+      <c r="B1" s="48"/>
+      <c r="C1" s="48"/>
+      <c r="D1" s="48"/>
+      <c r="E1" s="48"/>
+      <c r="F1" s="48"/>
     </row>
     <row r="2" spans="1:8">
       <c r="A2" s="18" t="s">
@@ -14956,7 +15860,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr enableFormatConditionsCalculation="0">
     <tabColor theme="7" tint="0.39997558519241921"/>
@@ -14977,16 +15881,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="24" customHeight="1">
-      <c r="A1" s="36" t="s">
+      <c r="A1" s="49" t="s">
         <v>263</v>
       </c>
-      <c r="B1" s="36"/>
-      <c r="C1" s="36"/>
-      <c r="D1" s="36"/>
-      <c r="E1" s="36"/>
-      <c r="F1" s="36"/>
-      <c r="G1" s="36"/>
-      <c r="H1" s="36"/>
+      <c r="B1" s="49"/>
+      <c r="C1" s="49"/>
+      <c r="D1" s="49"/>
+      <c r="E1" s="49"/>
+      <c r="F1" s="49"/>
+      <c r="G1" s="49"/>
+      <c r="H1" s="49"/>
     </row>
     <row r="2" spans="1:8" ht="28">
       <c r="A2" s="19" t="s">
@@ -15179,7 +16083,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr enableFormatConditionsCalculation="0">
     <tabColor rgb="FFFC8686"/>
@@ -15200,14 +16104,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="24" customHeight="1">
-      <c r="A1" s="37" t="s">
+      <c r="A1" s="50" t="s">
         <v>267</v>
       </c>
-      <c r="B1" s="37"/>
-      <c r="C1" s="37"/>
-      <c r="D1" s="37"/>
-      <c r="E1" s="37"/>
-      <c r="F1" s="37"/>
+      <c r="B1" s="50"/>
+      <c r="C1" s="50"/>
+      <c r="D1" s="50"/>
+      <c r="E1" s="50"/>
+      <c r="F1" s="50"/>
     </row>
     <row r="2" spans="1:6">
       <c r="A2" s="20" t="s">
@@ -16179,361 +17083,4 @@
     </ext>
   </extLst>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr enableFormatConditionsCalculation="0">
-    <tabColor theme="6" tint="0.39997558519241921"/>
-  </sheetPr>
-  <dimension ref="A1:E54"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E41" sqref="E41"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
-  <cols>
-    <col min="2" max="2" width="50.6640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="15.1640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="24.5" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="24" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:5">
-      <c r="A1" s="8" t="s">
-        <v>268</v>
-      </c>
-      <c r="B1" s="8"/>
-      <c r="C1" s="8"/>
-      <c r="D1" s="8"/>
-    </row>
-    <row r="2" spans="1:5">
-      <c r="A2" s="21" t="s">
-        <v>241</v>
-      </c>
-      <c r="B2" s="21" t="s">
-        <v>240</v>
-      </c>
-      <c r="C2" s="21" t="s">
-        <v>735</v>
-      </c>
-      <c r="D2" s="21" t="s">
-        <v>736</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" s="16" customFormat="1">
-      <c r="A3" s="16" t="s">
-        <v>276</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5">
-      <c r="B4" t="s">
-        <v>272</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5">
-      <c r="C5" s="22" t="s">
-        <v>6</v>
-      </c>
-      <c r="D5" t="s">
-        <v>737</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5">
-      <c r="C6" s="22" t="s">
-        <v>6</v>
-      </c>
-      <c r="D6" t="s">
-        <v>738</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5">
-      <c r="C7" s="22" t="s">
-        <v>6</v>
-      </c>
-      <c r="D7" t="s">
-        <v>739</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5">
-      <c r="C8" s="22" t="s">
-        <v>6</v>
-      </c>
-      <c r="D8" t="s">
-        <v>740</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5">
-      <c r="C9" s="22" t="s">
-        <v>6</v>
-      </c>
-      <c r="D9" t="s">
-        <v>741</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5">
-      <c r="C10" s="22" t="s">
-        <v>742</v>
-      </c>
-      <c r="D10" t="s">
-        <v>743</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5">
-      <c r="C11" s="22" t="s">
-        <v>742</v>
-      </c>
-      <c r="D11" t="s">
-        <v>744</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5">
-      <c r="C12" s="22" t="s">
-        <v>742</v>
-      </c>
-      <c r="D12" t="s">
-        <v>745</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5">
-      <c r="C13" s="22" t="s">
-        <v>742</v>
-      </c>
-      <c r="D13" t="s">
-        <v>746</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5">
-      <c r="C14" s="22" t="s">
-        <v>742</v>
-      </c>
-      <c r="D14" t="s">
-        <v>747</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5">
-      <c r="C15" s="22"/>
-    </row>
-    <row r="16" spans="1:5">
-      <c r="A16" s="21" t="s">
-        <v>241</v>
-      </c>
-      <c r="B16" s="21" t="s">
-        <v>240</v>
-      </c>
-      <c r="C16" s="21" t="s">
-        <v>0</v>
-      </c>
-      <c r="D16" s="21" t="s">
-        <v>570</v>
-      </c>
-      <c r="E16" s="21" t="s">
-        <v>749</v>
-      </c>
-    </row>
-    <row r="17" spans="2:4" s="16" customFormat="1">
-      <c r="B17" s="16" t="s">
-        <v>273</v>
-      </c>
-    </row>
-    <row r="18" spans="2:4">
-      <c r="C18" t="s">
-        <v>714</v>
-      </c>
-    </row>
-    <row r="19" spans="2:4">
-      <c r="D19" t="s">
-        <v>709</v>
-      </c>
-    </row>
-    <row r="20" spans="2:4">
-      <c r="D20" t="s">
-        <v>710</v>
-      </c>
-    </row>
-    <row r="21" spans="2:4">
-      <c r="C21" t="s">
-        <v>715</v>
-      </c>
-    </row>
-    <row r="22" spans="2:4">
-      <c r="D22" t="s">
-        <v>711</v>
-      </c>
-    </row>
-    <row r="23" spans="2:4">
-      <c r="D23" t="s">
-        <v>712</v>
-      </c>
-    </row>
-    <row r="24" spans="2:4">
-      <c r="C24" t="s">
-        <v>716</v>
-      </c>
-    </row>
-    <row r="25" spans="2:4">
-      <c r="D25" t="s">
-        <v>711</v>
-      </c>
-    </row>
-    <row r="26" spans="2:4">
-      <c r="D26" t="s">
-        <v>712</v>
-      </c>
-    </row>
-    <row r="27" spans="2:4">
-      <c r="C27" t="s">
-        <v>717</v>
-      </c>
-    </row>
-    <row r="28" spans="2:4">
-      <c r="D28" t="s">
-        <v>713</v>
-      </c>
-    </row>
-    <row r="29" spans="2:4">
-      <c r="D29" t="s">
-        <v>712</v>
-      </c>
-    </row>
-    <row r="30" spans="2:4">
-      <c r="C30" t="s">
-        <v>718</v>
-      </c>
-    </row>
-    <row r="31" spans="2:4">
-      <c r="D31" t="s">
-        <v>711</v>
-      </c>
-    </row>
-    <row r="32" spans="2:4">
-      <c r="D32" t="s">
-        <v>712</v>
-      </c>
-    </row>
-    <row r="33" spans="1:5">
-      <c r="E33" t="s">
-        <v>721</v>
-      </c>
-    </row>
-    <row r="34" spans="1:5">
-      <c r="E34" t="s">
-        <v>712</v>
-      </c>
-    </row>
-    <row r="35" spans="1:5">
-      <c r="E35" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="36" spans="1:5">
-      <c r="C36" t="s">
-        <v>719</v>
-      </c>
-    </row>
-    <row r="37" spans="1:5">
-      <c r="D37" t="s">
-        <v>720</v>
-      </c>
-    </row>
-    <row r="38" spans="1:5">
-      <c r="D38" t="s">
-        <v>712</v>
-      </c>
-    </row>
-    <row r="39" spans="1:5">
-      <c r="E39" t="s">
-        <v>722</v>
-      </c>
-    </row>
-    <row r="40" spans="1:5">
-      <c r="E40" t="s">
-        <v>723</v>
-      </c>
-    </row>
-    <row r="41" spans="1:5">
-      <c r="E41" t="s">
-        <v>724</v>
-      </c>
-    </row>
-    <row r="42" spans="1:5">
-      <c r="A42" s="21" t="s">
-        <v>241</v>
-      </c>
-      <c r="B42" s="21" t="s">
-        <v>240</v>
-      </c>
-      <c r="C42" s="21" t="s">
-        <v>0</v>
-      </c>
-      <c r="D42" s="21"/>
-    </row>
-    <row r="43" spans="1:5" s="16" customFormat="1">
-      <c r="B43" s="16" t="s">
-        <v>274</v>
-      </c>
-    </row>
-    <row r="44" spans="1:5">
-      <c r="C44" t="s">
-        <v>725</v>
-      </c>
-    </row>
-    <row r="45" spans="1:5">
-      <c r="C45" t="s">
-        <v>726</v>
-      </c>
-    </row>
-    <row r="46" spans="1:5">
-      <c r="C46" t="s">
-        <v>727</v>
-      </c>
-    </row>
-    <row r="47" spans="1:5">
-      <c r="C47" t="s">
-        <v>728</v>
-      </c>
-    </row>
-    <row r="48" spans="1:5">
-      <c r="C48" t="s">
-        <v>729</v>
-      </c>
-    </row>
-    <row r="49" spans="2:3">
-      <c r="C49" t="s">
-        <v>730</v>
-      </c>
-    </row>
-    <row r="50" spans="2:3">
-      <c r="C50" t="s">
-        <v>731</v>
-      </c>
-    </row>
-    <row r="51" spans="2:3">
-      <c r="C51" t="s">
-        <v>732</v>
-      </c>
-    </row>
-    <row r="52" spans="2:3">
-      <c r="C52" t="s">
-        <v>733</v>
-      </c>
-    </row>
-    <row r="54" spans="2:3" s="16" customFormat="1">
-      <c r="B54" s="16" t="s">
-        <v>275</v>
-      </c>
-      <c r="C54" s="16" t="s">
-        <v>734</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
-</worksheet>
 </file>
</xml_diff>